<commit_message>
there was no problem idiot
</commit_message>
<xml_diff>
--- a/2024 Project v2/data/generated/permit_price_to_Percentage_of_BAU_v1_1 - Excel.xlsx
+++ b/2024 Project v2/data/generated/permit_price_to_Percentage_of_BAU_v1_1 - Excel.xlsx
@@ -8,20 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kostas\Documents\GitHub\Diplomatiki_kwpap_step_1\2024 Project v2\data\generated\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{4066DBC9-A90A-451E-B6D0-3F3BCF42BF71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71981729-300E-401A-93BB-D2B13DB747A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="16305" activeTab="1" xr2:uid="{153B5B2A-F470-4B84-9EB6-E1A89CD34F14}"/>
+    <workbookView xWindow="7320" yWindow="0" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{153B5B2A-F470-4B84-9EB6-E1A89CD34F14}"/>
   </bookViews>
   <sheets>
     <sheet name="permit_price_to_Percentage_of_B" sheetId="1" r:id="rId1"/>
     <sheet name="Δοκιμή" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="297">
   <si>
     <t>Percentage of BAU</t>
   </si>
@@ -906,6 +919,12 @@
   </si>
   <si>
     <t>Correct?</t>
+  </si>
+  <si>
+    <t>1787.8315470249322</t>
+  </si>
+  <si>
+    <t>29.103830456733704</t>
   </si>
 </sst>
 </file>
@@ -1389,8 +1408,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Έμφαση1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3805,7 +3825,7 @@
   <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3865,22 +3885,22 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0.23232323232323199</v>
-      </c>
-      <c r="B2">
-        <v>520.50791875409402</v>
-      </c>
-      <c r="C2">
-        <v>112.777343019843</v>
+        <v>0.79797979797979801</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>296</v>
       </c>
       <c r="D2" t="s">
-        <v>75</v>
+        <v>222</v>
       </c>
       <c r="E2" t="s">
-        <v>76</v>
+        <v>223</v>
       </c>
       <c r="F2" t="s">
-        <v>77</v>
+        <v>224</v>
       </c>
       <c r="G2" t="s">
         <v>287</v>
@@ -3892,27 +3912,27 @@
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2</f>
-        <v>0.23232323232323199</v>
-      </c>
-      <c r="B3">
+        <v>0.79797979797979801</v>
+      </c>
+      <c r="B3" t="str">
         <f>B2</f>
-        <v>520.50791875409402</v>
-      </c>
-      <c r="C3">
+        <v>1787.8315470249322</v>
+      </c>
+      <c r="C3" t="str">
         <f>C2</f>
-        <v>112.777343019843</v>
+        <v>29.103830456733704</v>
       </c>
       <c r="D3">
         <f>--TRIM(LEFT(SUBSTITUTE(SUBSTITUTE(D2,"(",""),")",""), FIND(",", SUBSTITUTE(D2,"(",""))-1))</f>
-        <v>10.461748292376599</v>
+        <v>176.045234291263</v>
       </c>
       <c r="E3">
         <f>--TRIM(LEFT(SUBSTITUTE(SUBSTITUTE(E2,"(",""),")",""), FIND(",", SUBSTITUTE(E2,"(",""))-1))</f>
-        <v>4.0009999959999902</v>
+        <v>171.880422811263</v>
       </c>
       <c r="F3">
         <f>--TRIM(LEFT(SUBSTITUTE(SUBSTITUTE(F2,"(",""),")",""), FIND(",", SUBSTITUTE(F2,"(",""))-1))</f>
-        <v>510.56948741080902</v>
+        <v>3382.0140187186698</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -3922,57 +3942,57 @@
       </c>
       <c r="I3">
         <f>SUMIF(H:H, H3, D:D)</f>
-        <v>20.921727063648667</v>
+        <v>551.13103582769907</v>
       </c>
       <c r="J3">
         <f>100-0.1*I3</f>
-        <v>97.907827293635137</v>
+        <v>44.886896417230091</v>
       </c>
       <c r="K3">
         <f>D3*J3</f>
-        <v>1024.2870449994905</v>
+        <v>7902.1241963789253</v>
       </c>
       <c r="L3">
         <f>0.1*(D3-E3)^4+100/(E3)^2</f>
-        <v>180.48022619306133</v>
+        <v>30.090558482435171</v>
       </c>
       <c r="M3">
-        <f>2*(E3-A3*D3)</f>
-        <v>3.1409856339260118</v>
+        <f>C3*(E3-0.1*D3)</f>
+        <v>4490.0196191778141</v>
       </c>
       <c r="N3">
         <f>K3-L3-M3</f>
-        <v>840.6658331725032</v>
+        <v>3382.0140187186762</v>
       </c>
       <c r="O3">
         <f>ABS((N3-F3))/ABS(MAX(F3,N3))</f>
-        <v>0.39266059441951767</v>
+        <v>1.8824472273543449E-15</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A8" si="0">A3</f>
-        <v>0.23232323232323199</v>
-      </c>
-      <c r="B4">
+        <v>0.79797979797979801</v>
+      </c>
+      <c r="B4" t="str">
         <f t="shared" ref="B4:B8" si="1">B3</f>
-        <v>520.50791875409402</v>
-      </c>
-      <c r="C4">
+        <v>1787.8315470249322</v>
+      </c>
+      <c r="C4" t="str">
         <f t="shared" ref="C4:C8" si="2">C3</f>
-        <v>112.777343019843</v>
+        <v>29.103830456733704</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:E4" si="3">--TRIM(MID(SUBSTITUTE(SUBSTITUTE(D2,"(",""),")",""), FIND(",", D2) + 1, FIND(",", SUBSTITUTE(D2,"(",""), FIND(",", D2) + 1) - FIND(",", D2) - 1))</f>
-        <v>5.4074557422614902</v>
+        <v>187.542900768218</v>
       </c>
       <c r="E4">
         <f t="shared" si="3"/>
-        <v>3.0009999970000001</v>
+        <v>186.23139631536401</v>
       </c>
       <c r="F4">
         <f>--TRIM(MID(SUBSTITUTE(SUBSTITUTE(F2,"(",""),")",""), FIND(",", F2) + 1, FIND(",", SUBSTITUTE(F2,"(",""), FIND(",", F2) + 1) - FIND(",", F2) - 1))</f>
-        <v>164.47223345429799</v>
+        <v>3532.08445431993</v>
       </c>
       <c r="G4">
         <v>2</v>
@@ -3982,57 +4002,57 @@
       </c>
       <c r="I4">
         <f t="shared" ref="I4:I8" si="4">SUMIF(H:H, H4, D:D)</f>
-        <v>20.921727063648667</v>
+        <v>551.13103582769907</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J8" si="5">100-0.1*I4</f>
-        <v>97.907827293635137</v>
+        <f t="shared" ref="J4:J5" si="5">100-0.1*I4</f>
+        <v>44.886896417230091</v>
       </c>
       <c r="K4">
         <f t="shared" ref="K4:K8" si="6">D4*J4</f>
-        <v>529.43224291131355</v>
+        <v>8418.2187605698637</v>
       </c>
       <c r="L4">
         <f>5*(D4-E4)^3.2+40/(E4)^2</f>
-        <v>87.499052503762925</v>
+        <v>11.909000899002388</v>
       </c>
       <c r="M4">
-        <f>2*(E4-A4*D4)</f>
-        <v>3.4894448006259782</v>
+        <f>C4*(E4-0.1*D4)</f>
+        <v>4874.2253053509103</v>
       </c>
       <c r="N4">
         <f t="shared" ref="N4:N8" si="7">K4-L4-M4</f>
-        <v>438.44374560692467</v>
+        <v>3532.084454319951</v>
       </c>
       <c r="O4">
         <f t="shared" ref="O4:O8" si="8">ABS((N4-F4))/ABS(MAX(F4,N4))</f>
-        <v>0.62487266587273604</v>
+        <v>5.9223890060705992E-15</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
-        <v>0.23232323232323199</v>
-      </c>
-      <c r="B5">
+        <v>0.79797979797979801</v>
+      </c>
+      <c r="B5" t="str">
         <f t="shared" si="1"/>
-        <v>520.50791875409402</v>
-      </c>
-      <c r="C5">
+        <v>1787.8315470249322</v>
+      </c>
+      <c r="C5" t="str">
         <f t="shared" si="2"/>
-        <v>112.777343019843</v>
+        <v>29.103830456733704</v>
       </c>
       <c r="D5">
         <f t="shared" ref="D5:E5" si="9">--TRIM(MID(SUBSTITUTE(SUBSTITUTE(D2,"(",""),")",""), FIND(",", D2, FIND(",", D2) + 1) + 1, FIND(",", SUBSTITUTE(D2,"(",""), FIND(",", D2, FIND(",", D2) + 1) + 1) - FIND(",", D2, FIND(",", D2) + 1) - 1))</f>
-        <v>5.0525230290105796</v>
+        <v>187.542900768218</v>
       </c>
       <c r="E5">
         <f t="shared" si="9"/>
-        <v>3.0009999970000001</v>
+        <v>186.03266677179599</v>
       </c>
       <c r="F5">
         <f>--TRIM(MID(SUBSTITUTE(SUBSTITUTE(F2,"(",""),")",""), FIND(",", F2, FIND(",", F2) + 1) + 1, FIND(",", SUBSTITUTE(F2,"(",""), FIND(",", F2, FIND(",", F2) + 1) + 1) - FIND(",", F2, FIND(",", F2) + 1) - 1))</f>
-        <v>167.930338121479</v>
+        <v>3541.24478767337</v>
       </c>
       <c r="G5">
         <v>3</v>
@@ -4042,56 +4062,56 @@
       </c>
       <c r="I5">
         <f t="shared" si="4"/>
-        <v>20.921727063648667</v>
+        <v>551.13103582769907</v>
       </c>
       <c r="J5">
         <f t="shared" si="5"/>
-        <v>97.907827293635137</v>
+        <v>44.886896417230091</v>
       </c>
       <c r="K5">
         <f t="shared" si="6"/>
-        <v>494.68155212148207</v>
+        <v>8418.2187605698637</v>
       </c>
       <c r="L5">
         <f>(D5-E5)^5.2+30/(E5)^2</f>
-        <v>45.287420211624401</v>
+        <v>8.5324584883137788</v>
       </c>
       <c r="M5">
-        <f t="shared" ref="M5:M8" si="10">2*(E5-A5*D5)</f>
-        <v>3.6543630310253907</v>
+        <f>C5*(E5-0.1*D5)</f>
+        <v>4868.4415144081622</v>
       </c>
       <c r="N5">
         <f t="shared" si="7"/>
-        <v>445.73976887883225</v>
+        <v>3541.2447876733868</v>
       </c>
       <c r="O5">
         <f t="shared" si="8"/>
-        <v>0.62325475569776145</v>
+        <v>4.7513382981507183E-15</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="str">
         <f t="shared" si="1"/>
-        <v>520.50791875409402</v>
-      </c>
-      <c r="C6">
+        <v>1787.8315470249322</v>
+      </c>
+      <c r="C6" t="str">
         <f t="shared" si="2"/>
-        <v>112.777343019843</v>
+        <v>29.103830456733704</v>
       </c>
       <c r="D6">
-        <f t="shared" ref="D6:E6" si="11">--TRIM(MID(SUBSTITUTE(SUBSTITUTE(D2,"(",""),")",""), FIND(",", D2, FIND(",", D2, FIND(",", D2) + 1) + 1) + 1, FIND(",", SUBSTITUTE(D2,"(",""), FIND(",", D2, FIND(",", D2, FIND(",", D2) + 1) + 1) + 1) - FIND(",", D2, FIND(",", D2, FIND(",", D2) + 1) + 1) - 1))</f>
-        <v>106.12395594543</v>
+        <f t="shared" ref="D6:E6" si="10">--TRIM(MID(SUBSTITUTE(SUBSTITUTE(D2,"(",""),")",""), FIND(",", D2, FIND(",", D2, FIND(",", D2) + 1) + 1) + 1, FIND(",", SUBSTITUTE(D2,"(",""), FIND(",", D2, FIND(",", D2, FIND(",", D2) + 1) + 1) + 1) - FIND(",", D2, FIND(",", D2, FIND(",", D2) + 1) + 1) - 1))</f>
+        <v>292.03514691425198</v>
       </c>
       <c r="E6">
-        <f t="shared" si="11"/>
-        <v>101.53533006471299</v>
+        <f t="shared" si="10"/>
+        <v>289.47768714949598</v>
       </c>
       <c r="F6">
         <f>--TRIM(MID(SUBSTITUTE(SUBSTITUTE(F2,"(",""),")",""), FIND(",", F2, FIND(",", F2, FIND(",", F2) + 1) + 1) + 1, FIND(",", SUBSTITUTE(F2,"(",""), FIND(",", F2, FIND(",", F2, FIND(",", F2) + 1) + 1) + 1) - FIND(",", F2, FIND(",", F2, FIND(",", F2) + 1) + 1) - 1))</f>
-        <v>1534.8380140957099</v>
+        <v>9083.7998342921001</v>
       </c>
       <c r="G6">
         <v>4</v>
@@ -4101,31 +4121,31 @@
       </c>
       <c r="I6">
         <f t="shared" si="4"/>
-        <v>318.37186783628999</v>
+        <v>914.25157609014605</v>
       </c>
       <c r="J6">
         <f>150-0.1*I6</f>
-        <v>118.16281321637101</v>
+        <v>58.574842390985395</v>
       </c>
       <c r="K6">
         <f t="shared" si="6"/>
-        <v>12539.905184162229</v>
+        <v>17105.912703130576</v>
       </c>
       <c r="L6">
         <f>(D6-E6)^3.3+20/(E6)^2</f>
-        <v>152.60131183940754</v>
+        <v>22.170411192124131</v>
       </c>
       <c r="M6">
-        <f t="shared" si="10"/>
-        <v>203.07066012942599</v>
+        <f>C6*(E6-0.05*D6)</f>
+        <v>7999.9424576463452</v>
       </c>
       <c r="N6">
         <f t="shared" si="7"/>
-        <v>12184.233212193396</v>
+        <v>9083.7998342921055</v>
       </c>
       <c r="O6">
         <f t="shared" si="8"/>
-        <v>0.87403080790018706</v>
+        <v>6.0073628989897566E-16</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -4133,25 +4153,25 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="str">
         <f t="shared" si="1"/>
-        <v>520.50791875409402</v>
-      </c>
-      <c r="C7">
+        <v>1787.8315470249322</v>
+      </c>
+      <c r="C7" t="str">
         <f t="shared" si="2"/>
-        <v>112.777343019843</v>
+        <v>29.103830456733704</v>
       </c>
       <c r="D7">
-        <f t="shared" ref="D7:E7" si="12">--TRIM(MID(SUBSTITUTE(SUBSTITUTE(D2,"(",""),")",""), FIND(",", D2, FIND(",", D2, FIND(",", D2, FIND(",", D2) + 1) + 1) + 1) + 1, FIND(",", SUBSTITUTE(D2,"(",""), FIND(",", D2, FIND(",", D2, FIND(",", D2, FIND(",", D2) + 1) + 1) + 1) + 1) - FIND(",", D2, FIND(",", D2, FIND(",", D2, FIND(",", D2) + 1) + 1) + 1) - 1))</f>
-        <v>106.12395594543</v>
+        <f t="shared" ref="D7:E7" si="11">--TRIM(MID(SUBSTITUTE(SUBSTITUTE(D2,"(",""),")",""), FIND(",", D2, FIND(",", D2, FIND(",", D2, FIND(",", D2) + 1) + 1) + 1) + 1, FIND(",", SUBSTITUTE(D2,"(",""), FIND(",", D2, FIND(",", D2, FIND(",", D2, FIND(",", D2) + 1) + 1) + 1) + 1) - FIND(",", D2, FIND(",", D2, FIND(",", D2, FIND(",", D2) + 1) + 1) + 1) - 1))</f>
+        <v>311.10821458794697</v>
       </c>
       <c r="E7">
-        <f t="shared" si="12"/>
-        <v>86.278777093425006</v>
+        <f t="shared" si="11"/>
+        <v>304.05767139970402</v>
       </c>
       <c r="F7">
         <f>--TRIM(MID(SUBSTITUTE(SUBSTITUTE(F2,"(",""),")",""), FIND(",", F2, FIND(",", F2, FIND(",", F2, FIND(",", F2) + 1) + 1) + 1) + 1, FIND(",", SUBSTITUTE(F2,"(",""), FIND(",", F2, FIND(",", F2, FIND(",", F2, FIND(",", F2) + 1) + 1) + 1) + 1) - FIND(",", F2, FIND(",", F2, FIND(",", F2, FIND(",", F2) + 1) + 1) + 1) - 1))</f>
-        <v>2442.8540902607901</v>
+        <v>9737.2811042743997</v>
       </c>
       <c r="G7">
         <v>5</v>
@@ -4161,31 +4181,31 @@
       </c>
       <c r="I7">
         <f t="shared" si="4"/>
-        <v>318.37186783628999</v>
+        <v>914.25157609014605</v>
       </c>
       <c r="J7">
-        <f t="shared" ref="J7:J8" si="13">150-0.1*I7</f>
-        <v>118.16281321637101</v>
+        <f t="shared" ref="J7:J8" si="12">150-0.1*I7</f>
+        <v>58.574842390985395</v>
       </c>
       <c r="K7">
         <f t="shared" si="6"/>
-        <v>12539.905184162229</v>
+        <v>18223.114636029859</v>
       </c>
       <c r="L7">
         <f>(D7-E7)^2.3+20/(E7)^2</f>
-        <v>965.17874341767856</v>
+        <v>89.312650822442123</v>
       </c>
       <c r="M7">
-        <f t="shared" si="10"/>
-        <v>172.55755418685001</v>
+        <f>C7*(E7-0.05*D7)</f>
+        <v>8396.5208809329961</v>
       </c>
       <c r="N7">
         <f t="shared" si="7"/>
-        <v>11402.168886557702</v>
+        <v>9737.2811042744215</v>
       </c>
       <c r="O7">
         <f t="shared" si="8"/>
-        <v>0.78575531422440781</v>
+        <v>2.2416804659124396E-15</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -4193,25 +4213,25 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B8">
+      <c r="B8" t="str">
         <f t="shared" si="1"/>
-        <v>520.50791875409402</v>
-      </c>
-      <c r="C8">
+        <v>1787.8315470249322</v>
+      </c>
+      <c r="C8" t="str">
         <f t="shared" si="2"/>
-        <v>112.777343019843</v>
+        <v>29.103830456733704</v>
       </c>
       <c r="D8">
-        <f t="shared" ref="D8:E8" si="14">--TRIM(MID(SUBSTITUTE(SUBSTITUTE(D2,"(",""),")",""), FIND(",", D2, FIND(",", D2, FIND(",", D2, FIND(",", D2, FIND(",", D2) + 1) + 1) + 1) + 1) + 1, FIND(",", SUBSTITUTE(D2,"(",""), FIND(",", D2, FIND(",", D2, FIND(",", D2, FIND(",", D2, FIND(",", D2) + 1) + 1) + 1) + 1) + 1) - FIND(",", D2, FIND(",", D2, FIND(",", D2, FIND(",", D2, FIND(",", D2) + 1) + 1) + 1) + 1) - 1))</f>
-        <v>106.12395594543</v>
+        <f t="shared" ref="D8:E8" si="13">--TRIM(MID(SUBSTITUTE(SUBSTITUTE(D2,"(",""),")",""), FIND(",", D2, FIND(",", D2, FIND(",", D2, FIND(",", D2, FIND(",", D2) + 1) + 1) + 1) + 1) + 1, FIND(",", SUBSTITUTE(D2,"(",""), FIND(",", D2, FIND(",", D2, FIND(",", D2, FIND(",", D2, FIND(",", D2) + 1) + 1) + 1) + 1) + 1) - FIND(",", D2, FIND(",", D2, FIND(",", D2, FIND(",", D2, FIND(",", D2) + 1) + 1) + 1) + 1) - 1))</f>
+        <v>311.10821458794697</v>
       </c>
       <c r="E8">
-        <f t="shared" si="14"/>
-        <v>101.07080064061</v>
+        <f t="shared" si="13"/>
+        <v>308.35425711055899</v>
       </c>
       <c r="F8">
         <f>--TRIM(MID(SUBSTITUTE(SUBSTITUTE(F2,"(",""),")",""), FIND(",", F2, FIND(",", F2, FIND(",", F2, FIND(",", F2, FIND(",", F2) + 1) + 1) + 1) + 1) + 1, FIND(",", SUBSTITUTE(F2,"(",""), FIND(",", F2, FIND(",", F2, FIND(",", F2, FIND(",", F2, FIND(",", F2) + 1) + 1) + 1) + 1) + 1) - FIND(",", F2, FIND(",", F2, FIND(",", F2, FIND(",", F2, FIND(",", F2) + 1) + 1) + 1) + 1) - 1))</f>
-        <v>1561.4239441218001</v>
+        <v>9675.96869823821</v>
       </c>
       <c r="G8">
         <v>6</v>
@@ -4221,31 +4241,31 @@
       </c>
       <c r="I8">
         <f t="shared" si="4"/>
-        <v>318.37186783628999</v>
+        <v>914.25157609014605</v>
       </c>
       <c r="J8">
-        <f t="shared" si="13"/>
-        <v>118.16281321637101</v>
+        <f t="shared" si="12"/>
+        <v>58.574842390985395</v>
       </c>
       <c r="K8">
         <f t="shared" si="6"/>
-        <v>12539.905184162229</v>
+        <v>18223.114636029859</v>
       </c>
       <c r="L8">
         <f>(D8-E8)^3.2+15/(E8)^2</f>
-        <v>178.40377601819495</v>
+        <v>25.577954787084856</v>
       </c>
       <c r="M8">
-        <f t="shared" si="10"/>
-        <v>202.14160128122001</v>
+        <f>C8*(E8-0.05*D8)</f>
+        <v>8521.5679830045447</v>
       </c>
       <c r="N8">
         <f t="shared" si="7"/>
-        <v>12159.359806862814</v>
+        <v>9675.96869823823</v>
       </c>
       <c r="O8">
         <f t="shared" si="8"/>
-        <v>0.871586665011712</v>
+        <v>2.0678946018756321E-15</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>